<commit_message>
Power BI + HTML Resume
</commit_message>
<xml_diff>
--- a/PowerBI_Projects/Resume_powerBI/data.xlsx
+++ b/PowerBI_Projects/Resume_powerBI/data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivana\Google Drive\CURSO DATA SCIENCE\Github\Data Analysis\Curriculum_powerBI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\GITHUB\Data-Analysis-Projects\PowerBI_Projects\Resume_powerBI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA19FF2-CA95-4620-982B-38DA88BD821C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFFA339-2FD1-416A-8A01-C80F8DC42F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{B97437BD-7417-45F9-B287-770D6BA39F14}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{B97437BD-7417-45F9-B287-770D6BA39F14}"/>
   </bookViews>
   <sheets>
     <sheet name="Skills" sheetId="1" r:id="rId1"/>
     <sheet name="Languages" sheetId="3" r:id="rId2"/>
     <sheet name="Education" sheetId="2" r:id="rId3"/>
     <sheet name="JOBS" sheetId="4" r:id="rId4"/>
+    <sheet name="Images" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Skills!$A$1:$H$25</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>Power BI</t>
   </si>
@@ -184,6 +185,15 @@
   </si>
   <si>
     <t>Organization</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1jOFJwGX8ve_L_ZODyOZEO2WP2nLvSVRE/view</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>img</t>
   </si>
 </sst>
 </file>
@@ -529,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -539,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213B0822-0127-4BA7-A441-8D5194BB1572}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26:H26"/>
     </sheetView>
   </sheetViews>
@@ -1246,4 +1256,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F337495B-E50B-4391-8E8A-9BCAB6897CF8}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>